<commit_message>
Lastenheft nach Bergmann kommis
</commit_message>
<xml_diff>
--- a/Projektleitfaden/Meilensteinplan/Meilensteinplan_02052020.xlsx
+++ b/Projektleitfaden/Meilensteinplan/Meilensteinplan_02052020.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HannesDittmann/Documents/Studium/Master Business and Systems Engineering/3.Semester/Masterarbeit/Dokumente/Master_Doc/Präsentationen/Meilensteinplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HannesDittmann/Documents/Studium/Master Business and Systems Engineering/3.Semester/Masterarbeit/Dokumente/Master_Doc/Projektleitfaden/Meilensteinplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20180" tabRatio="179"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20140" tabRatio="179"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>AKTIVITÄT</t>
   </si>
@@ -157,22 +157,7 @@
     </r>
   </si>
   <si>
-    <t>MS 2: Konzeptphase</t>
-  </si>
-  <si>
     <t>MS 0: Einarbeitung</t>
-  </si>
-  <si>
-    <t>MS 3: ROS</t>
-  </si>
-  <si>
-    <t>MS 4: Modellbasierte Entwicklung (Matlab/Simulink)</t>
-  </si>
-  <si>
-    <t>MS 5: Verifikation</t>
-  </si>
-  <si>
-    <t>MS 6: Validierung</t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
@@ -205,22 +190,40 @@
     <t>Einarbeitung Spracherkennung in Matlab/Simulink und Code-Generierung</t>
   </si>
   <si>
-    <t>Konzeptionierung Spracherkennung</t>
+    <t>Anforderungserhebung und Testspezifikationen</t>
   </si>
   <si>
-    <t>Konzeptionierung Personenerkennung und Tracking</t>
+    <t xml:space="preserve">Einarbeitung Spracherkennung </t>
   </si>
   <si>
-    <t>Konzeptionierung Betriebsmodi</t>
+    <t>Einarbeitung Personenerkennung</t>
   </si>
   <si>
-    <t>Konzeptionierung Post-Processing statische Karte</t>
+    <t>MS 2: Implementierung</t>
   </si>
   <si>
-    <t>MS 7: Implementierungsdokumentation/Masterarbeit/HSHL-Wiki</t>
+    <t>Implementierung Spracherkennung</t>
   </si>
   <si>
-    <t>Anforderungserhebung und Testspezifikationen</t>
+    <t>Implementierung Personenerkennung und Tracking</t>
+  </si>
+  <si>
+    <t>Implementierung State Machine</t>
+  </si>
+  <si>
+    <t>MS 3: Verfikation und Validierung</t>
+  </si>
+  <si>
+    <t>Verifikation und Validierung</t>
+  </si>
+  <si>
+    <t>Konzeptionierung Gesamtsystem</t>
+  </si>
+  <si>
+    <t>MS 4: Implementierungsdokumentation</t>
+  </si>
+  <si>
+    <t>Implementierungsdokumentation</t>
   </si>
 </sst>
 </file>
@@ -643,7 +646,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,8 +715,20 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,15 +810,6 @@
     <xf numFmtId="9" fontId="6" fillId="12" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="6" fillId="14" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -813,9 +819,6 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="11" xfId="19" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="19" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -858,6 +861,51 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="12" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -879,62 +927,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="12" borderId="0" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="28">
     <cellStyle name="% abgeschlossen" xfId="16"/>
     <cellStyle name="Aktivität" xfId="2"/>
     <cellStyle name="Akzent1" xfId="19" builtinId="29"/>
     <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Bezeichnung" xfId="5"/>
     <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15"/>
     <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18"/>
     <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17"/>
@@ -1127,7 +1134,7 @@
         <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{062CB36E-7785-4A4E-BD87-687703FCF4EE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{062CB36E-7785-4A4E-BD87-687703FCF4EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1387,13 +1394,13 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO49"/>
+  <dimension ref="B1:BO44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18:B21"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1416,7 @@
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="18"/>
       <c r="D1" s="23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1420,115 +1427,115 @@
       <c r="D2" s="23"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="65">
+      <c r="H2" s="54">
+        <v>17</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="58" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="62"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="51"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="67" t="s">
+      <c r="AA2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
+      <c r="AO2" s="45"/>
+      <c r="AP2" s="45"/>
     </row>
     <row r="3" spans="2:67" ht="14" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="66"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="62"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="55"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="45"/>
+      <c r="Y3" s="51"/>
       <c r="Z3" s="17"/>
-      <c r="AA3" s="55" t="s">
+      <c r="AA3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="56"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
+      <c r="AB3" s="45"/>
+      <c r="AC3" s="45"/>
+      <c r="AD3" s="45"/>
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45"/>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="45"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="45"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="45"/>
+      <c r="AM3" s="45"/>
+      <c r="AN3" s="45"/>
+      <c r="AO3" s="45"/>
+      <c r="AP3" s="45"/>
     </row>
     <row r="4" spans="2:67" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="64" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="13" t="s">
@@ -1536,9 +1543,9 @@
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
@@ -1554,117 +1561,117 @@
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
       <c r="AD4" s="10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:67" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="49"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="31">
+      <c r="B5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="28">
         <v>10</v>
       </c>
       <c r="I5" s="8">
         <v>11</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="28">
         <v>12</v>
       </c>
       <c r="K5" s="8">
         <v>13</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="28">
         <v>14</v>
       </c>
       <c r="M5" s="8">
         <v>15</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="28">
         <v>16</v>
       </c>
       <c r="O5" s="8">
         <v>17</v>
       </c>
-      <c r="P5" s="31">
+      <c r="P5" s="28">
         <v>18</v>
       </c>
       <c r="Q5" s="8">
         <v>19</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="28">
         <v>20</v>
       </c>
       <c r="S5" s="8">
         <v>21</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="28">
         <v>22</v>
       </c>
       <c r="U5" s="8">
         <v>23</v>
       </c>
-      <c r="V5" s="31">
+      <c r="V5" s="28">
         <v>24</v>
       </c>
       <c r="W5" s="8">
         <v>25</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="28">
         <v>26</v>
       </c>
       <c r="Y5" s="8">
         <v>27</v>
       </c>
-      <c r="Z5" s="31">
+      <c r="Z5" s="28">
         <v>28</v>
       </c>
       <c r="AA5" s="8">
         <v>29</v>
       </c>
-      <c r="AB5" s="31">
+      <c r="AB5" s="28">
         <v>30</v>
       </c>
       <c r="AC5" s="8">
         <v>31</v>
       </c>
-      <c r="AD5" s="31">
+      <c r="AD5" s="28">
         <v>32</v>
       </c>
       <c r="AE5" s="8">
         <v>33</v>
       </c>
-      <c r="AF5" s="31">
+      <c r="AF5" s="28">
         <v>34</v>
       </c>
       <c r="AG5" s="8">
         <v>35</v>
       </c>
-      <c r="AH5" s="31">
+      <c r="AH5" s="28">
         <v>36</v>
       </c>
       <c r="AI5" s="8">
         <v>37</v>
       </c>
-      <c r="AJ5" s="31">
+      <c r="AJ5" s="28">
         <v>38</v>
       </c>
       <c r="AK5" s="8">
         <v>39</v>
       </c>
-      <c r="AL5" s="31">
+      <c r="AL5" s="28">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:67" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="49"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="53"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="64"/>
       <c r="H6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1687,15 +1694,15 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
-      <c r="AC6" s="47"/>
+      <c r="AC6" s="43"/>
     </row>
     <row r="7" spans="2:67" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="50"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="54"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="3">
         <v>1</v>
       </c>
@@ -1759,7 +1766,7 @@
       <c r="AB7" s="3">
         <v>21</v>
       </c>
-      <c r="AC7" s="46">
+      <c r="AC7" s="42">
         <v>22</v>
       </c>
       <c r="AD7" s="3">
@@ -1878,19 +1885,19 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="43">
+      <c r="B8" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="39">
         <v>1</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="39">
         <v>1</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="39">
         <v>1</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="39">
         <v>1</v>
       </c>
       <c r="G8" s="24">
@@ -1917,7 +1924,7 @@
       <c r="Z8" s="20"/>
       <c r="AA8" s="20"/>
       <c r="AB8" s="21"/>
-      <c r="AC8" s="35"/>
+      <c r="AC8" s="31"/>
       <c r="AD8" s="21"/>
       <c r="AE8" s="22"/>
       <c r="AF8" s="22"/>
@@ -1958,19 +1965,19 @@
       <c r="BO8" s="22"/>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="43">
+      <c r="B9" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="39">
         <v>2</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="39">
         <v>1</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="39">
         <v>1</v>
       </c>
       <c r="G9" s="24">
@@ -1997,7 +2004,7 @@
       <c r="Z9" s="20"/>
       <c r="AA9" s="20"/>
       <c r="AB9" s="21"/>
-      <c r="AC9" s="35"/>
+      <c r="AC9" s="31"/>
       <c r="AD9" s="21"/>
       <c r="AE9" s="22"/>
       <c r="AF9" s="22"/>
@@ -2038,19 +2045,19 @@
       <c r="BO9" s="22"/>
     </row>
     <row r="10" spans="2:67" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="43">
+      <c r="B10" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="39">
         <v>3</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="39">
         <v>1</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="39">
         <v>3</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="39">
         <v>2</v>
       </c>
       <c r="G10" s="24">
@@ -2077,7 +2084,7 @@
       <c r="Z10" s="20"/>
       <c r="AA10" s="20"/>
       <c r="AB10" s="21"/>
-      <c r="AC10" s="35"/>
+      <c r="AC10" s="31"/>
       <c r="AD10" s="21"/>
       <c r="AE10" s="22"/>
       <c r="AF10" s="22"/>
@@ -2118,19 +2125,19 @@
       <c r="BO10" s="22"/>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="43">
+      <c r="B11" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="39">
         <v>4</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="39">
         <v>1</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="39">
         <v>5</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="39">
         <v>1</v>
       </c>
       <c r="G11" s="24">
@@ -2157,7 +2164,7 @@
       <c r="Z11" s="20"/>
       <c r="AA11" s="20"/>
       <c r="AB11" s="21"/>
-      <c r="AC11" s="35"/>
+      <c r="AC11" s="31"/>
       <c r="AD11" s="21"/>
       <c r="AE11" s="22"/>
       <c r="AF11" s="22"/>
@@ -2198,19 +2205,19 @@
       <c r="BO11" s="22"/>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="43">
+      <c r="B12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="39">
         <v>5</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="39">
         <v>1</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="39">
         <v>6</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="39">
         <v>1</v>
       </c>
       <c r="G12" s="24">
@@ -2237,7 +2244,7 @@
       <c r="Z12" s="20"/>
       <c r="AA12" s="20"/>
       <c r="AB12" s="21"/>
-      <c r="AC12" s="35"/>
+      <c r="AC12" s="31"/>
       <c r="AD12" s="21"/>
       <c r="AE12" s="22"/>
       <c r="AF12" s="22"/>
@@ -2278,23 +2285,23 @@
       <c r="BO12" s="22"/>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="43">
+      <c r="B13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="39">
         <v>6</v>
       </c>
-      <c r="D13" s="43">
-        <v>2</v>
-      </c>
-      <c r="E13" s="43">
+      <c r="D13" s="39">
+        <v>3</v>
+      </c>
+      <c r="E13" s="39">
         <v>7</v>
       </c>
-      <c r="F13" s="43" t="s">
-        <v>23</v>
+      <c r="F13" s="39">
+        <v>3</v>
       </c>
       <c r="G13" s="24">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -2317,7 +2324,7 @@
       <c r="Z13" s="20"/>
       <c r="AA13" s="20"/>
       <c r="AB13" s="21"/>
-      <c r="AC13" s="35"/>
+      <c r="AC13" s="31"/>
       <c r="AD13" s="21"/>
       <c r="AE13" s="22"/>
       <c r="AF13" s="22"/>
@@ -2358,23 +2365,23 @@
       <c r="BO13" s="22"/>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="43">
+      <c r="B14" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="39">
+        <v>7</v>
+      </c>
+      <c r="D14" s="39">
+        <v>6</v>
+      </c>
+      <c r="E14" s="39">
         <v>8</v>
       </c>
-      <c r="D14" s="43">
+      <c r="F14" s="39">
+        <v>6</v>
+      </c>
+      <c r="G14" s="24">
         <v>1</v>
-      </c>
-      <c r="E14" s="43">
-        <v>9</v>
-      </c>
-      <c r="F14" s="43">
-        <v>1</v>
-      </c>
-      <c r="G14" s="24">
-        <v>0.5</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -2397,7 +2404,7 @@
       <c r="Z14" s="20"/>
       <c r="AA14" s="20"/>
       <c r="AB14" s="21"/>
-      <c r="AC14" s="32"/>
+      <c r="AC14" s="31"/>
       <c r="AD14" s="21"/>
       <c r="AE14" s="22"/>
       <c r="AF14" s="22"/>
@@ -2438,22 +2445,22 @@
       <c r="BO14" s="22"/>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="44">
-        <v>1</v>
-      </c>
-      <c r="D15" s="44">
-        <v>9</v>
-      </c>
-      <c r="E15" s="44">
-        <v>1</v>
-      </c>
-      <c r="F15" s="44">
-        <v>9</v>
-      </c>
-      <c r="G15" s="26">
+      <c r="B15" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="39">
+        <v>7</v>
+      </c>
+      <c r="D15" s="39">
+        <v>6</v>
+      </c>
+      <c r="E15" s="39">
+        <v>8</v>
+      </c>
+      <c r="F15" s="39">
+        <v>6</v>
+      </c>
+      <c r="G15" s="24">
         <v>1</v>
       </c>
       <c r="H15" s="20"/>
@@ -2477,7 +2484,7 @@
       <c r="Z15" s="20"/>
       <c r="AA15" s="20"/>
       <c r="AB15" s="21"/>
-      <c r="AC15" s="32"/>
+      <c r="AC15" s="31"/>
       <c r="AD15" s="21"/>
       <c r="AE15" s="22"/>
       <c r="AF15" s="22"/>
@@ -2518,20 +2525,20 @@
       <c r="BO15" s="22"/>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="43">
-        <v>5</v>
-      </c>
-      <c r="D16" s="43">
-        <v>4</v>
-      </c>
-      <c r="E16" s="43">
-        <v>7</v>
-      </c>
-      <c r="F16" s="43" t="s">
+      <c r="B16" s="36" t="s">
         <v>23</v>
+      </c>
+      <c r="C16" s="39">
+        <v>10</v>
+      </c>
+      <c r="D16" s="39">
+        <v>1</v>
+      </c>
+      <c r="E16" s="39">
+        <v>11</v>
+      </c>
+      <c r="F16" s="39">
+        <v>1</v>
       </c>
       <c r="G16" s="24">
         <v>0</v>
@@ -2557,7 +2564,7 @@
       <c r="Z16" s="20"/>
       <c r="AA16" s="20"/>
       <c r="AB16" s="21"/>
-      <c r="AC16" s="32"/>
+      <c r="AC16" s="31"/>
       <c r="AD16" s="21"/>
       <c r="AE16" s="22"/>
       <c r="AF16" s="22"/>
@@ -2598,22 +2605,24 @@
       <c r="BO16" s="22"/>
     </row>
     <row r="17" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="44">
-        <v>5</v>
-      </c>
-      <c r="D17" s="44">
-        <v>4</v>
-      </c>
-      <c r="E17" s="44">
-        <v>7</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="26"/>
+      <c r="B17" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="40">
+        <v>1</v>
+      </c>
+      <c r="D17" s="40">
+        <v>14</v>
+      </c>
+      <c r="E17" s="40">
+        <v>1</v>
+      </c>
+      <c r="F17" s="40">
+        <v>15</v>
+      </c>
+      <c r="G17" s="26">
+        <v>1</v>
+      </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -2635,7 +2644,7 @@
       <c r="Z17" s="20"/>
       <c r="AA17" s="20"/>
       <c r="AB17" s="21"/>
-      <c r="AC17" s="32"/>
+      <c r="AC17" s="29"/>
       <c r="AD17" s="21"/>
       <c r="AE17" s="22"/>
       <c r="AF17" s="22"/>
@@ -2676,15 +2685,23 @@
       <c r="BO17" s="22"/>
     </row>
     <row r="18" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
+      <c r="B18" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="39">
+        <v>14</v>
+      </c>
+      <c r="D18" s="39">
+        <v>3</v>
+      </c>
+      <c r="E18" s="39">
+        <v>14</v>
+      </c>
+      <c r="F18" s="39">
+        <v>3</v>
+      </c>
       <c r="G18" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
@@ -2707,7 +2724,7 @@
       <c r="Z18" s="20"/>
       <c r="AA18" s="20"/>
       <c r="AB18" s="21"/>
-      <c r="AC18" s="32"/>
+      <c r="AC18" s="29"/>
       <c r="AD18" s="21"/>
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
@@ -2748,14 +2765,24 @@
       <c r="BO18" s="22"/>
     </row>
     <row r="19" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="24"/>
+      <c r="B19" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="39">
+        <v>15</v>
+      </c>
+      <c r="D19" s="39">
+        <v>2</v>
+      </c>
+      <c r="E19" s="39">
+        <v>15</v>
+      </c>
+      <c r="F19" s="39">
+        <v>2</v>
+      </c>
+      <c r="G19" s="24">
+        <v>1</v>
+      </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
@@ -2777,7 +2804,7 @@
       <c r="Z19" s="20"/>
       <c r="AA19" s="20"/>
       <c r="AB19" s="21"/>
-      <c r="AC19" s="32"/>
+      <c r="AC19" s="29"/>
       <c r="AD19" s="21"/>
       <c r="AE19" s="22"/>
       <c r="AF19" s="22"/>
@@ -2818,14 +2845,24 @@
       <c r="BO19" s="22"/>
     </row>
     <row r="20" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="24"/>
+      <c r="B20" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="40">
+        <v>14</v>
+      </c>
+      <c r="D20" s="40">
+        <v>3</v>
+      </c>
+      <c r="E20" s="40">
+        <v>14</v>
+      </c>
+      <c r="F20" s="40">
+        <v>3</v>
+      </c>
+      <c r="G20" s="26">
+        <v>1</v>
+      </c>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -2847,7 +2884,7 @@
       <c r="Z20" s="20"/>
       <c r="AA20" s="20"/>
       <c r="AB20" s="21"/>
-      <c r="AC20" s="32"/>
+      <c r="AC20" s="29"/>
       <c r="AD20" s="21"/>
       <c r="AE20" s="22"/>
       <c r="AF20" s="22"/>
@@ -2888,15 +2925,23 @@
       <c r="BO20" s="22"/>
     </row>
     <row r="21" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="B21" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="39">
+        <v>14</v>
+      </c>
+      <c r="D21" s="39">
+        <v>5</v>
+      </c>
+      <c r="E21" s="39">
+        <v>14</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>18</v>
+      </c>
       <c r="G21" s="24">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
@@ -2919,7 +2964,7 @@
       <c r="Z21" s="20"/>
       <c r="AA21" s="20"/>
       <c r="AB21" s="21"/>
-      <c r="AC21" s="32"/>
+      <c r="AC21" s="29"/>
       <c r="AD21" s="21"/>
       <c r="AE21" s="22"/>
       <c r="AF21" s="22"/>
@@ -2960,16 +3005,24 @@
       <c r="BO21" s="22"/>
     </row>
     <row r="22" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="44">
-        <v>10</v>
-      </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="26"/>
+      <c r="B22" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="39">
+        <v>14</v>
+      </c>
+      <c r="D22" s="39">
+        <v>5</v>
+      </c>
+      <c r="E22" s="39">
+        <v>14</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0.8</v>
+      </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
@@ -2991,7 +3044,7 @@
       <c r="Z22" s="20"/>
       <c r="AA22" s="20"/>
       <c r="AB22" s="21"/>
-      <c r="AC22" s="32"/>
+      <c r="AC22" s="29"/>
       <c r="AD22" s="21"/>
       <c r="AE22" s="22"/>
       <c r="AF22" s="22"/>
@@ -3032,11 +3085,21 @@
       <c r="BO22" s="22"/>
     </row>
     <row r="23" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="40"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
+      <c r="B23" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="39">
+        <v>19</v>
+      </c>
+      <c r="D23" s="39">
+        <v>4</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>18</v>
+      </c>
       <c r="G23" s="24">
         <v>0</v>
       </c>
@@ -3061,7 +3124,7 @@
       <c r="Z23" s="20"/>
       <c r="AA23" s="20"/>
       <c r="AB23" s="21"/>
-      <c r="AC23" s="32"/>
+      <c r="AC23" s="29"/>
       <c r="AD23" s="21"/>
       <c r="AE23" s="22"/>
       <c r="AF23" s="22"/>
@@ -3102,13 +3165,23 @@
       <c r="BO23" s="22"/>
     </row>
     <row r="24" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="40"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="24">
-        <v>0</v>
+      <c r="B24" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="40">
+        <v>14</v>
+      </c>
+      <c r="D24" s="40">
+        <v>9</v>
+      </c>
+      <c r="E24" s="40">
+        <v>14</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0.5</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
@@ -3131,7 +3204,7 @@
       <c r="Z24" s="20"/>
       <c r="AA24" s="20"/>
       <c r="AB24" s="21"/>
-      <c r="AC24" s="32"/>
+      <c r="AC24" s="29"/>
       <c r="AD24" s="21"/>
       <c r="AE24" s="22"/>
       <c r="AF24" s="22"/>
@@ -3172,14 +3245,24 @@
       <c r="BO24" s="22"/>
     </row>
     <row r="25" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="39">
+        <v>23</v>
+      </c>
+      <c r="D25" s="39">
+        <v>4</v>
+      </c>
+      <c r="E25" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="24">
+        <v>0</v>
+      </c>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
@@ -3201,7 +3284,7 @@
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="21"/>
-      <c r="AC25" s="32"/>
+      <c r="AC25" s="29"/>
       <c r="AD25" s="21"/>
       <c r="AE25" s="22"/>
       <c r="AF25" s="22"/>
@@ -3242,14 +3325,22 @@
       <c r="BO25" s="22"/>
     </row>
     <row r="26" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="40"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43" t="s">
+      <c r="B26" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="40">
         <v>23</v>
       </c>
-      <c r="G26" s="24">
+      <c r="D26" s="40">
+        <v>4</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="26">
         <v>0</v>
       </c>
       <c r="H26" s="20"/>
@@ -3273,7 +3364,7 @@
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
       <c r="AB26" s="21"/>
-      <c r="AC26" s="32"/>
+      <c r="AC26" s="29"/>
       <c r="AD26" s="21"/>
       <c r="AE26" s="22"/>
       <c r="AF26" s="22"/>
@@ -3314,11 +3405,21 @@
       <c r="BO26" s="22"/>
     </row>
     <row r="27" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="40"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
+      <c r="B27" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="39">
+        <v>27</v>
+      </c>
+      <c r="D27" s="39">
+        <v>8</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>18</v>
+      </c>
       <c r="G27" s="24">
         <v>0</v>
       </c>
@@ -3343,7 +3444,7 @@
       <c r="Z27" s="20"/>
       <c r="AA27" s="20"/>
       <c r="AB27" s="21"/>
-      <c r="AC27" s="32"/>
+      <c r="AC27" s="29"/>
       <c r="AD27" s="21"/>
       <c r="AE27" s="22"/>
       <c r="AF27" s="22"/>
@@ -3384,320 +3485,224 @@
       <c r="BO27" s="22"/>
     </row>
     <row r="28" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="40"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="24">
+      <c r="B28" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="40">
+        <v>27</v>
+      </c>
+      <c r="D28" s="40">
+        <v>8</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="26">
         <v>0</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20"/>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20"/>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="21"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="21"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22"/>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="22"/>
-      <c r="AT28" s="22"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22"/>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="22"/>
-      <c r="BC28" s="22"/>
-      <c r="BD28" s="22"/>
-      <c r="BE28" s="22"/>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22"/>
-      <c r="BL28" s="22"/>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
+      <c r="AC28" s="30"/>
     </row>
     <row r="29" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="40"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="24">
-        <v>0</v>
-      </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="28"/>
-      <c r="AC29" s="33"/>
-      <c r="AD29" s="28"/>
-      <c r="AE29" s="29"/>
-      <c r="AF29" s="29"/>
-      <c r="AG29" s="29"/>
-      <c r="AH29" s="29"/>
-      <c r="AI29" s="29"/>
-      <c r="AJ29" s="29"/>
-      <c r="AK29" s="29"/>
-      <c r="AL29" s="29"/>
-      <c r="AM29" s="29"/>
-      <c r="AN29" s="29"/>
-      <c r="AO29" s="29"/>
-      <c r="AP29" s="29"/>
-      <c r="AQ29" s="29"/>
-      <c r="AR29" s="29"/>
-      <c r="AS29" s="29"/>
-      <c r="AT29" s="29"/>
-      <c r="AU29" s="29"/>
-      <c r="AV29" s="29"/>
-      <c r="AW29" s="29"/>
-      <c r="AX29" s="29"/>
-      <c r="AY29" s="29"/>
-      <c r="AZ29" s="29"/>
-      <c r="BA29" s="29"/>
-      <c r="BB29" s="29"/>
-      <c r="BC29" s="29"/>
-      <c r="BD29" s="29"/>
-      <c r="BE29" s="29"/>
-      <c r="BF29" s="29"/>
-      <c r="BG29" s="29"/>
-      <c r="BH29" s="29"/>
-      <c r="BI29" s="29"/>
-      <c r="BJ29" s="29"/>
-      <c r="BK29" s="29"/>
-      <c r="BL29" s="29"/>
-      <c r="BM29" s="29"/>
-      <c r="BN29" s="29"/>
-      <c r="BO29" s="29"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="24"/>
+      <c r="AC29" s="30"/>
     </row>
     <row r="30" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="26"/>
-      <c r="AC30" s="34"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="24"/>
+      <c r="AC30" s="30"/>
     </row>
     <row r="31" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="40"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="24">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="34"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="27"/>
+      <c r="AC31" s="30"/>
     </row>
     <row r="32" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="40"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="24">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="34"/>
-    </row>
-    <row r="33" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="26"/>
-      <c r="AC33" s="34"/>
-    </row>
-    <row r="34" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="42"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="34"/>
-    </row>
-    <row r="35" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="26"/>
-      <c r="AC35" s="34"/>
-    </row>
-    <row r="36" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="40"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="26"/>
-    </row>
-    <row r="38" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="25"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="24"/>
-    </row>
-    <row r="39" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="25"/>
-      <c r="C39" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="25"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="24"/>
-    </row>
-    <row r="41" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="25"/>
-      <c r="C41" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="36"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="25"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="25"/>
+      <c r="C34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="25"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="25"/>
+      <c r="C36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="24"/>
-    </row>
-    <row r="43" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>10</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>10</v>
       </c>
@@ -3734,111 +3739,18 @@
         <v>10</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="2:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="7" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
     <mergeCell ref="AI3:AP3"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="K3:O3"/>
@@ -3852,16 +3764,9 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="AI2:AP2"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="H8:BO49">
+  <conditionalFormatting sqref="H8:BO44">
     <cfRule type="expression" dxfId="9" priority="9">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
@@ -3884,7 +3789,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:BO50">
+  <conditionalFormatting sqref="B45:BO45">
     <cfRule type="expression" dxfId="2" priority="10">
       <formula>TRUE</formula>
     </cfRule>
@@ -3894,7 +3799,7 @@
       <formula>H$7=Zeitraum_ausgewählt</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BO49">
+  <conditionalFormatting sqref="H7:BO44">
     <cfRule type="expression" dxfId="0" priority="15">
       <formula>H$7=Zeitraum_ausgewählt</formula>
     </cfRule>

</xml_diff>